<commit_message>
Fiche 1 - Fin
</commit_message>
<xml_diff>
--- a/Gestion des riques.xlsx
+++ b/Gestion des riques.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenthardouin/Documents/L2 INFO/Projet_GL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{8CA95728-AC68-D24B-8F33-ECF5A19461B8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917A616-E079-434A-9AB3-8530BFEE51D9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="460" windowWidth="24640" windowHeight="13640" xr2:uid="{4C3F2B6B-390C-1549-940C-1F9F01709E6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$B$1:$G$17</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Nature</t>
   </si>
@@ -63,9 +66,6 @@
     <t>Manque de compétence pour une tâche</t>
   </si>
   <si>
-    <t>moyen</t>
-  </si>
-  <si>
     <t>Retard à prévoir</t>
   </si>
   <si>
@@ -90,9 +90,6 @@
     <t>Mauvaise expression du besoin</t>
   </si>
   <si>
-    <t>faible</t>
-  </si>
-  <si>
     <t>Tâche qui n'est pas ce qui était attendu</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>Non connaissance utilisation Framework</t>
   </si>
   <si>
-    <t>forte</t>
-  </si>
-  <si>
     <t>projet pas possible sans certains framework</t>
   </si>
   <si>
@@ -178,13 +172,19 @@
   </si>
   <si>
     <t>Gestion des risques</t>
+  </si>
+  <si>
+    <t>Moyen</t>
+  </si>
+  <si>
+    <t>Forte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +200,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -207,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +233,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -236,29 +255,118 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="40 % - Accent3" xfId="3" builtinId="39"/>
+    <cellStyle name="60 % - Accent3" xfId="4" builtinId="40"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1 univ" xfId="1" xr:uid="{7A2E3F21-CD34-2645-8ABC-A7F1C99C80EA}"/>
     <cellStyle name="Style 2 univ" xfId="2" xr:uid="{033F4D08-8530-8E42-99E3-705A0FC2FE4E}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -274,7 +382,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{314668B4-31B9-9A41-85C5-CE7B8D544587}" name="Tableau1" displayName="Tableau1" ref="B4:G16" totalsRowShown="0" headerRowCellStyle="Style 2 univ" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{314668B4-31B9-9A41-85C5-CE7B8D544587}" name="Tableau1" displayName="Tableau1" ref="B4:G16" totalsRowShown="0" tableBorderDxfId="1" headerRowCellStyle="Style 2 univ" dataCellStyle="Normal">
   <autoFilter ref="B4:G16" xr:uid="{B138E44E-CEA4-7C4C-B1FE-F0CAC1ABA64C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E4D53506-6D40-B04F-8817-317388895287}" name="Nature" dataCellStyle="Normal"/>
@@ -284,7 +392,7 @@
     <tableColumn id="5" xr3:uid="{7DC904F1-6E51-0D4D-9B61-E18288CBCC3E}" name="Impacts" dataCellStyle="Normal"/>
     <tableColumn id="6" xr3:uid="{C50B7A14-D582-E248-8906-0276F58145B5}" name="Action de réduction des risques" dataCellStyle="Normal"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -588,10 +696,10 @@
   <dimension ref="B1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="44.1640625" customWidth="1"/>
@@ -601,279 +709,302 @@
     <col min="7" max="7" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
+    <row r="1" spans="2:7" ht="25" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="2:7">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="2:7">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2">
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="4">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="8">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="F15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="6">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="2">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3</v>
-      </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="2">
-        <v>3</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="F16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2">
-        <v>3</v>
-      </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>
   </mergeCells>
+  <conditionalFormatting sqref="D5:D16">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Moyen">
+      <formula>NOT(ISERROR(SEARCH("Moyen",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Faible">
+      <formula>NOT(ISERROR(SEARCH("Faible",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Forte">
+      <formula>NOT(ISERROR(SEARCH("Forte",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E16">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="2"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>